<commit_message>
Add notes about application build requirements
</commit_message>
<xml_diff>
--- a/content/learning-paths/servers-and-cloud-computing/profiling-for-neoverse/reports/v1-spe.xlsx
+++ b/content/learning-paths/servers-and-cloud-computing/profiling-for-neoverse/reports/v1-spe.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julgas01/git/arm-learning-paths/content/learning-paths/servers-and-cloud-computing/profiling-for-neoverse/reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9178F0-F5CF-2B40-9E3E-6036B803888B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="220" yWindow="1120" windowWidth="30020" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Function</t>
   </si>
@@ -118,11 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,96 +467,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="24" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="27" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="28" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="29" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="30" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="31" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="44" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="45" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="46" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="47" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="48" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="49" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="50" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="24" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="27" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="28" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="30" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="31" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="44" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="45" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="46" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="47" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="48" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="49" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="50" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U13" totalsRowShown="0">
-  <autoFilter ref="A1:U13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U13" totalsRowShown="0">
+  <autoFilter ref="A1:U13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="21">
-    <tableColumn id="1" name="Function"/>
-    <tableColumn id="2" name="Samples"/>
-    <tableColumn id="3" name="Samples%"/>
-    <tableColumn id="4" name="CPI"/>
-    <tableColumn id="5" name="Retiring%"/>
-    <tableColumn id="6" name="FE bound%"/>
-    <tableColumn id="7" name="Bad spec%"/>
-    <tableColumn id="8" name="BE bound%"/>
-    <tableColumn id="9" name="L1I$ M%"/>
-    <tableColumn id="10" name="L1I$ MPKI"/>
-    <tableColumn id="11" name="Branch M%"/>
-    <tableColumn id="12" name="Branch MPKI"/>
-    <tableColumn id="13" name="L1D$ M%"/>
-    <tableColumn id="14" name="L1D$ MPKI"/>
-    <tableColumn id="15" name="L2$ M%"/>
-    <tableColumn id="16" name="L2$ MPKI"/>
-    <tableColumn id="17" name="Int Op%"/>
-    <tableColumn id="18" name="FP Op%"/>
-    <tableColumn id="19" name="SIMD Op%"/>
-    <tableColumn id="20" name="Ld Op%"/>
-    <tableColumn id="21" name="St Op%"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Function"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Samples"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Samples%"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CPI"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Retiring%"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FE bound%"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Bad spec%"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="BE bound%"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="L1I$ M%"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="L1I$ MPKI"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Branch M%"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Branch MPKI"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="L1D$ M%"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="L1D$ MPKI"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="L2$ M%"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="L2$ MPKI"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Int Op%"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="FP Op%"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="SIMD Op%"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ld Op%"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="St Op%"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -591,7 +602,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -625,6 +636,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -659,9 +671,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -834,37 +847,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -937,64 +952,64 @@
         <v>1536145</v>
       </c>
       <c r="C2" s="3">
-        <v>24.4217</v>
+        <v>24.421700000000001</v>
       </c>
       <c r="D2" s="3">
         <v>1.22756</v>
       </c>
       <c r="E2" s="4">
-        <v>11.0606</v>
+        <v>11.060600000000001</v>
       </c>
       <c r="F2" s="3">
         <v>25.9253</v>
       </c>
       <c r="G2" s="5">
-        <v>33.2961</v>
+        <v>33.296100000000003</v>
       </c>
       <c r="H2" s="3">
-        <v>29.6064</v>
+        <v>29.606400000000001</v>
       </c>
       <c r="I2" s="3">
-        <v>0.859531</v>
+        <v>0.85953100000000004</v>
       </c>
       <c r="J2" s="3">
-        <v>5.31163</v>
+        <v>5.3116300000000001</v>
       </c>
       <c r="K2" s="5">
         <v>21.27</v>
       </c>
       <c r="L2" s="5">
-        <v>23.1095</v>
+        <v>23.109500000000001</v>
       </c>
       <c r="M2" s="3">
-        <v>1.3293</v>
+        <v>1.3292999999999999</v>
       </c>
       <c r="N2" s="3">
-        <v>3.64918</v>
+        <v>3.6491799999999999</v>
       </c>
       <c r="O2" s="6">
-        <v>6.88787</v>
+        <v>6.8878700000000004</v>
       </c>
       <c r="P2" s="3">
         <v>1.22923</v>
       </c>
       <c r="Q2" s="3">
-        <v>18.647</v>
+        <v>18.646999999999998</v>
       </c>
       <c r="R2" s="3">
-        <v>20.3778</v>
+        <v>20.377800000000001</v>
       </c>
       <c r="S2" s="7">
-        <v>36.2552</v>
+        <v>36.255200000000002</v>
       </c>
       <c r="T2" s="3">
         <v>12.6027</v>
       </c>
       <c r="U2" s="3">
-        <v>0.261023</v>
+        <v>0.26102300000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1005,61 +1020,61 @@
         <v>12.3245</v>
       </c>
       <c r="D3" s="3">
-        <v>0.6161140000000001</v>
+        <v>0.61611400000000005</v>
       </c>
       <c r="E3" s="8">
-        <v>23.676</v>
+        <v>23.675999999999998</v>
       </c>
       <c r="F3" s="3">
         <v>28.03</v>
       </c>
       <c r="G3" s="9">
-        <v>15.6176</v>
+        <v>15.617599999999999</v>
       </c>
       <c r="H3" s="3">
-        <v>32.569</v>
+        <v>32.569000000000003</v>
       </c>
       <c r="I3" s="3">
-        <v>0.059135</v>
+        <v>5.9135E-2</v>
       </c>
       <c r="J3" s="3">
-        <v>0.150603</v>
+        <v>0.15060299999999999</v>
       </c>
       <c r="K3" s="10">
-        <v>12.296</v>
+        <v>12.295999999999999</v>
       </c>
       <c r="L3" s="11">
-        <v>6.14765</v>
+        <v>6.1476499999999996</v>
       </c>
       <c r="M3" s="3">
         <v>2.68676</v>
       </c>
       <c r="N3" s="12">
-        <v>8.47932</v>
+        <v>8.4793199999999995</v>
       </c>
       <c r="O3" s="13">
-        <v>5.41122</v>
+        <v>5.4112200000000001</v>
       </c>
       <c r="P3" s="3">
         <v>1.13866</v>
       </c>
       <c r="Q3" s="14">
-        <v>43.1397</v>
+        <v>43.139699999999998</v>
       </c>
       <c r="R3" s="3">
         <v>0</v>
       </c>
       <c r="S3" s="15">
-        <v>25.8623</v>
+        <v>25.862300000000001</v>
       </c>
       <c r="T3" s="3">
-        <v>25.1928</v>
+        <v>25.192799999999998</v>
       </c>
       <c r="U3" s="3">
-        <v>0.613803</v>
+        <v>0.61380299999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1067,64 +1082,64 @@
         <v>707509</v>
       </c>
       <c r="C4" s="3">
-        <v>11.248</v>
+        <v>11.247999999999999</v>
       </c>
       <c r="D4" s="3">
-        <v>0.531038</v>
+        <v>0.53103800000000001</v>
       </c>
       <c r="E4" s="3">
-        <v>26.4811</v>
+        <v>26.481100000000001</v>
       </c>
       <c r="F4" s="16">
-        <v>40.254</v>
+        <v>40.253999999999998</v>
       </c>
       <c r="G4" s="3">
-        <v>7.55638</v>
+        <v>7.5563799999999999</v>
       </c>
       <c r="H4" s="3">
-        <v>25.5568</v>
+        <v>25.556799999999999</v>
       </c>
       <c r="I4" s="3">
-        <v>0.200948</v>
+        <v>0.20094799999999999</v>
       </c>
       <c r="J4" s="3">
-        <v>0.379198</v>
+        <v>0.37919799999999998</v>
       </c>
       <c r="K4" s="3">
         <v>1.0319</v>
       </c>
       <c r="L4" s="3">
-        <v>0.13164</v>
+        <v>0.13164000000000001</v>
       </c>
       <c r="M4" s="3">
-        <v>0.8468560000000001</v>
+        <v>0.84685600000000005</v>
       </c>
       <c r="N4" s="3">
-        <v>2.85139</v>
+        <v>2.8513899999999999</v>
       </c>
       <c r="O4" s="17">
-        <v>11.1461</v>
+        <v>11.146100000000001</v>
       </c>
       <c r="P4" s="3">
-        <v>1.00849</v>
+        <v>1.0084900000000001</v>
       </c>
       <c r="Q4" s="18">
-        <v>41.5421</v>
+        <v>41.542099999999998</v>
       </c>
       <c r="R4" s="3">
-        <v>0.0201433</v>
+        <v>2.0143299999999999E-2</v>
       </c>
       <c r="S4" s="19">
         <v>29.0838</v>
       </c>
       <c r="T4" s="3">
-        <v>27.7406</v>
+        <v>27.740600000000001</v>
       </c>
       <c r="U4" s="3">
-        <v>0.08049630000000001</v>
+        <v>8.0496300000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1150,7 @@
         <v>10.8047</v>
       </c>
       <c r="D5" s="3">
-        <v>0.618665</v>
+        <v>0.61866500000000002</v>
       </c>
       <c r="E5" s="20">
         <v>21.0839</v>
@@ -1144,13 +1159,13 @@
         <v>31.7209</v>
       </c>
       <c r="G5" s="3">
-        <v>10.2504</v>
+        <v>10.250400000000001</v>
       </c>
       <c r="H5" s="3">
         <v>36.9099</v>
       </c>
       <c r="I5" s="3">
-        <v>0.06681960000000001</v>
+        <v>6.6819600000000007E-2</v>
       </c>
       <c r="J5" s="3">
         <v>0.149537</v>
@@ -1159,28 +1174,28 @@
         <v>10.2844</v>
       </c>
       <c r="L5" s="23">
-        <v>5.11502</v>
+        <v>5.1150200000000003</v>
       </c>
       <c r="M5" s="3">
-        <v>1.98924</v>
+        <v>1.9892399999999999</v>
       </c>
       <c r="N5" s="3">
-        <v>3.00268</v>
+        <v>3.0026799999999998</v>
       </c>
       <c r="O5" s="24">
-        <v>9.759180000000001</v>
+        <v>9.7591800000000006</v>
       </c>
       <c r="P5" s="3">
-        <v>0.686497</v>
+        <v>0.68649700000000002</v>
       </c>
       <c r="Q5" s="3">
         <v>21.3506</v>
       </c>
       <c r="R5" s="3">
-        <v>4.63484</v>
+        <v>4.6348399999999996</v>
       </c>
       <c r="S5" s="3">
-        <v>55.2734</v>
+        <v>55.273400000000002</v>
       </c>
       <c r="T5" s="3">
         <v>10.7502</v>
@@ -1189,7 +1204,7 @@
         <v>2.96787</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1197,64 +1212,64 @@
         <v>610515</v>
       </c>
       <c r="C6" s="3">
-        <v>9.70598</v>
+        <v>9.7059800000000003</v>
       </c>
       <c r="D6" s="3">
-        <v>0.699384</v>
+        <v>0.69938400000000001</v>
       </c>
       <c r="E6" s="22">
-        <v>19.7645</v>
+        <v>19.764500000000002</v>
       </c>
       <c r="F6" s="3">
-        <v>29.5952</v>
+        <v>29.595199999999998</v>
       </c>
       <c r="G6" s="3">
-        <v>9.96003</v>
+        <v>9.9600299999999997</v>
       </c>
       <c r="H6" s="3">
-        <v>40.5472</v>
+        <v>40.547199999999997</v>
       </c>
       <c r="I6" s="3">
-        <v>1.36156</v>
+        <v>1.3615600000000001</v>
       </c>
       <c r="J6" s="3">
-        <v>2.87166</v>
+        <v>2.8716599999999999</v>
       </c>
       <c r="K6" s="5">
         <v>46.6267</v>
       </c>
       <c r="L6" s="25">
-        <v>6.36594</v>
+        <v>6.3659400000000002</v>
       </c>
       <c r="M6" s="3">
-        <v>0.530865</v>
+        <v>0.53086500000000003</v>
       </c>
       <c r="N6" s="3">
-        <v>0.992213</v>
+        <v>0.99221300000000001</v>
       </c>
       <c r="O6" s="26">
-        <v>9.966900000000001</v>
+        <v>9.9669000000000008</v>
       </c>
       <c r="P6" s="3">
-        <v>0.759953</v>
+        <v>0.75995299999999999</v>
       </c>
       <c r="Q6" s="3">
-        <v>23.005</v>
+        <v>23.004999999999999</v>
       </c>
       <c r="R6" s="3">
-        <v>0.7783910000000001</v>
+        <v>0.77839100000000006</v>
       </c>
       <c r="S6" s="3">
-        <v>58.1273</v>
+        <v>58.127299999999998</v>
       </c>
       <c r="T6" s="3">
-        <v>15.9288</v>
+        <v>15.928800000000001</v>
       </c>
       <c r="U6" s="3">
         <v>0.723248</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1262,37 +1277,37 @@
         <v>317605</v>
       </c>
       <c r="C7" s="3">
-        <v>5.04929</v>
+        <v>5.0492900000000001</v>
       </c>
       <c r="D7" s="3">
-        <v>0.55375</v>
+        <v>0.55374999999999996</v>
       </c>
       <c r="E7" s="13">
-        <v>24.6558</v>
+        <v>24.655799999999999</v>
       </c>
       <c r="F7" s="27">
-        <v>32.3743</v>
+        <v>32.374299999999998</v>
       </c>
       <c r="G7" s="3">
-        <v>10.9904</v>
+        <v>10.990399999999999</v>
       </c>
       <c r="H7" s="3">
-        <v>31.2649</v>
+        <v>31.264900000000001</v>
       </c>
       <c r="I7" s="3">
-        <v>0.701807</v>
+        <v>0.70180699999999996</v>
       </c>
       <c r="J7" s="3">
         <v>1.49915</v>
       </c>
       <c r="K7" s="28">
-        <v>5.26761</v>
+        <v>5.2676100000000003</v>
       </c>
       <c r="L7" s="3">
-        <v>2.24845</v>
+        <v>2.2484500000000001</v>
       </c>
       <c r="M7" s="3">
-        <v>0.67516</v>
+        <v>0.67515999999999998</v>
       </c>
       <c r="N7" s="3">
         <v>1.26654</v>
@@ -1307,19 +1322,19 @@
         <v>55.0045</v>
       </c>
       <c r="R7" s="3">
-        <v>2.65677</v>
+        <v>2.6567699999999999</v>
       </c>
       <c r="S7" s="31">
-        <v>21.1079</v>
+        <v>21.107900000000001</v>
       </c>
       <c r="T7" s="3">
-        <v>10.6125</v>
+        <v>10.612500000000001</v>
       </c>
       <c r="U7" s="3">
-        <v>5.03895</v>
+        <v>5.0389499999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1330,61 +1345,61 @@
         <v>4.9051</v>
       </c>
       <c r="D8" s="3">
-        <v>0.744221</v>
+        <v>0.74422100000000002</v>
       </c>
       <c r="E8" s="32">
-        <v>16.5785</v>
+        <v>16.578499999999998</v>
       </c>
       <c r="F8" s="3">
         <v>25.9528</v>
       </c>
       <c r="G8" s="33">
-        <v>19.2162</v>
+        <v>19.216200000000001</v>
       </c>
       <c r="H8" s="3">
-        <v>37.9262</v>
+        <v>37.926200000000001</v>
       </c>
       <c r="I8" s="3">
-        <v>0.175421</v>
+        <v>0.17542099999999999</v>
       </c>
       <c r="J8" s="3">
-        <v>0.536056</v>
+        <v>0.53605599999999998</v>
       </c>
       <c r="K8" s="25">
-        <v>6.35733</v>
+        <v>6.3573300000000001</v>
       </c>
       <c r="L8" s="34">
-        <v>6.10929</v>
+        <v>6.1092899999999997</v>
       </c>
       <c r="M8" s="3">
-        <v>1.43592</v>
+        <v>1.4359200000000001</v>
       </c>
       <c r="N8" s="3">
         <v>4.72811</v>
       </c>
       <c r="O8" s="14">
-        <v>9.098560000000001</v>
+        <v>9.0985600000000009</v>
       </c>
       <c r="P8" s="3">
-        <v>1.10139</v>
+        <v>1.1013900000000001</v>
       </c>
       <c r="Q8" s="35">
-        <v>40.7138</v>
+        <v>40.713799999999999</v>
       </c>
       <c r="R8" s="3">
         <v>11.8736</v>
       </c>
       <c r="S8" s="36">
-        <v>14.5354</v>
+        <v>14.535399999999999</v>
       </c>
       <c r="T8" s="3">
-        <v>16.2924</v>
+        <v>16.292400000000001</v>
       </c>
       <c r="U8" s="3">
-        <v>5.87206</v>
+        <v>5.8720600000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1392,19 +1407,19 @@
         <v>287281</v>
       </c>
       <c r="C9" s="3">
-        <v>4.5672</v>
+        <v>4.5671999999999997</v>
       </c>
       <c r="D9" s="3">
-        <v>0.5306070000000001</v>
+        <v>0.53060700000000005</v>
       </c>
       <c r="E9" s="3">
-        <v>25.8722</v>
+        <v>25.872199999999999</v>
       </c>
       <c r="F9" s="37">
         <v>33.6571</v>
       </c>
       <c r="G9" s="3">
-        <v>8.38367</v>
+        <v>8.3836700000000004</v>
       </c>
       <c r="H9" s="3">
         <v>31.974</v>
@@ -1413,43 +1428,43 @@
         <v>0.18214</v>
       </c>
       <c r="J9" s="3">
-        <v>0.35238</v>
+        <v>0.35238000000000003</v>
       </c>
       <c r="K9" s="38">
-        <v>7.24454</v>
+        <v>7.2445399999999998</v>
       </c>
       <c r="L9" s="3">
         <v>2.4899</v>
       </c>
       <c r="M9" s="3">
-        <v>0.679094</v>
+        <v>0.67909399999999998</v>
       </c>
       <c r="N9" s="3">
-        <v>1.49684</v>
+        <v>1.4968399999999999</v>
       </c>
       <c r="O9" s="39">
         <v>17.5246</v>
       </c>
       <c r="P9" s="3">
-        <v>0.859258</v>
+        <v>0.85925799999999997</v>
       </c>
       <c r="Q9" s="3">
-        <v>25.1916</v>
+        <v>25.191600000000001</v>
       </c>
       <c r="R9" s="3">
-        <v>16.4256</v>
+        <v>16.425599999999999</v>
       </c>
       <c r="S9" s="40">
-        <v>34.915</v>
+        <v>34.914999999999999</v>
       </c>
       <c r="T9" s="3">
-        <v>19.353</v>
+        <v>19.353000000000002</v>
       </c>
       <c r="U9" s="3">
-        <v>0.574333</v>
+        <v>0.57433299999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1457,25 +1472,25 @@
         <v>233871</v>
       </c>
       <c r="C10" s="3">
-        <v>3.71809</v>
+        <v>3.7180900000000001</v>
       </c>
       <c r="D10" s="3">
         <v>1.48336</v>
       </c>
       <c r="E10" s="5">
-        <v>8.668710000000001</v>
+        <v>8.6687100000000008</v>
       </c>
       <c r="F10" s="3">
-        <v>25.0401</v>
+        <v>25.040099999999999</v>
       </c>
       <c r="G10" s="3">
-        <v>7.26158</v>
+        <v>7.2615800000000004</v>
       </c>
       <c r="H10" s="41">
-        <v>58.2458</v>
+        <v>58.245800000000003</v>
       </c>
       <c r="I10" s="3">
-        <v>0.708774</v>
+        <v>0.70877400000000002</v>
       </c>
       <c r="J10" s="3">
         <v>1.99926</v>
@@ -1484,37 +1499,37 @@
         <v>15.6069</v>
       </c>
       <c r="L10" s="43">
-        <v>7.15511</v>
+        <v>7.1551099999999996</v>
       </c>
       <c r="M10" s="3">
-        <v>2.82115</v>
+        <v>2.8211499999999998</v>
       </c>
       <c r="N10" s="3">
-        <v>4.95713</v>
+        <v>4.9571300000000003</v>
       </c>
       <c r="O10" s="5">
         <v>29.01</v>
       </c>
       <c r="P10" s="44">
-        <v>6.53211</v>
+        <v>6.5321100000000003</v>
       </c>
       <c r="Q10" s="3">
         <v>15.3409</v>
       </c>
       <c r="R10" s="3">
-        <v>2.45613</v>
+        <v>2.4561299999999999</v>
       </c>
       <c r="S10" s="3">
-        <v>64.7668</v>
+        <v>64.766800000000003</v>
       </c>
       <c r="T10" s="3">
-        <v>7.93529</v>
+        <v>7.9352900000000002</v>
       </c>
       <c r="U10" s="3">
-        <v>5.03717</v>
+        <v>5.0371699999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1522,64 +1537,64 @@
         <v>222131</v>
       </c>
       <c r="C11" s="3">
-        <v>3.53144</v>
+        <v>3.5314399999999999</v>
       </c>
       <c r="D11" s="3">
-        <v>0.746635</v>
+        <v>0.74663500000000005</v>
       </c>
       <c r="E11" s="45">
         <v>17.544</v>
       </c>
       <c r="F11" s="3">
-        <v>25.1634</v>
+        <v>25.163399999999999</v>
       </c>
       <c r="G11" s="3">
-        <v>8.2646</v>
+        <v>8.2645999999999997</v>
       </c>
       <c r="H11" s="25">
-        <v>48.9744</v>
+        <v>48.974400000000003</v>
       </c>
       <c r="I11" s="3">
-        <v>0.209336</v>
+        <v>0.20933599999999999</v>
       </c>
       <c r="J11" s="3">
         <v>0.457901</v>
       </c>
       <c r="K11" s="44">
-        <v>6.57793</v>
+        <v>6.5779300000000003</v>
       </c>
       <c r="L11" s="3">
-        <v>4.98803</v>
+        <v>4.9880300000000002</v>
       </c>
       <c r="M11" s="3">
-        <v>0.781842</v>
+        <v>0.78184200000000004</v>
       </c>
       <c r="N11" s="3">
         <v>1.53698</v>
       </c>
       <c r="O11" s="5">
-        <v>24.2198</v>
+        <v>24.219799999999999</v>
       </c>
       <c r="P11" s="3">
         <v>1.00518</v>
       </c>
       <c r="Q11" s="3">
-        <v>18.8803</v>
+        <v>18.880299999999998</v>
       </c>
       <c r="R11" s="3">
         <v>0.595468</v>
       </c>
       <c r="S11" s="3">
-        <v>56.5521</v>
+        <v>56.552100000000003</v>
       </c>
       <c r="T11" s="3">
         <v>14.8561</v>
       </c>
       <c r="U11" s="3">
-        <v>1.56997</v>
+        <v>1.5699700000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1590,13 +1605,13 @@
         <v>2.49777</v>
       </c>
       <c r="D12" s="3">
-        <v>0.475048</v>
+        <v>0.47504800000000003</v>
       </c>
       <c r="E12" s="46">
-        <v>23.2752</v>
+        <v>23.275200000000002</v>
       </c>
       <c r="F12" s="3">
-        <v>28.764</v>
+        <v>28.763999999999999</v>
       </c>
       <c r="G12" s="3">
         <v>12.5029</v>
@@ -1605,46 +1620,46 @@
         <v>35.7027</v>
       </c>
       <c r="I12" s="3">
-        <v>0.646367</v>
+        <v>0.64636700000000002</v>
       </c>
       <c r="J12" s="3">
         <v>1.20889</v>
       </c>
       <c r="K12" s="3">
-        <v>0.986826</v>
+        <v>0.98682599999999998</v>
       </c>
       <c r="L12" s="3">
-        <v>1.51621</v>
+        <v>1.5162100000000001</v>
       </c>
       <c r="M12" s="3">
-        <v>2.68991</v>
+        <v>2.6899099999999998</v>
       </c>
       <c r="N12" s="18">
-        <v>8.280279999999999</v>
+        <v>8.2802799999999994</v>
       </c>
       <c r="O12" s="38">
-        <v>7.17327</v>
+        <v>7.1732699999999996</v>
       </c>
       <c r="P12" s="3">
         <v>1.45966</v>
       </c>
       <c r="Q12" s="47">
-        <v>52.6842</v>
+        <v>52.684199999999997</v>
       </c>
       <c r="R12" s="3">
-        <v>0.820728</v>
+        <v>0.82072800000000001</v>
       </c>
       <c r="S12" s="5">
-        <v>7.39005</v>
+        <v>7.3900499999999996</v>
       </c>
       <c r="T12" s="3">
         <v>16.0639</v>
       </c>
       <c r="U12" s="3">
-        <v>8.277979999999999</v>
+        <v>8.2779799999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1655,62 +1670,63 @@
         <v>1.91821</v>
       </c>
       <c r="D13" s="3">
-        <v>0.458743</v>
+        <v>0.45874300000000001</v>
       </c>
       <c r="E13" s="3">
-        <v>31.5678</v>
+        <v>31.567799999999998</v>
       </c>
       <c r="F13" s="48">
-        <v>35.4203</v>
+        <v>35.420299999999997</v>
       </c>
       <c r="G13" s="3">
-        <v>8.279909999999999</v>
+        <v>8.2799099999999992</v>
       </c>
       <c r="H13" s="3">
         <v>24.6417</v>
       </c>
       <c r="I13" s="3">
-        <v>0.0309442</v>
+        <v>3.0944200000000002E-2</v>
       </c>
       <c r="J13" s="3">
-        <v>0.0576867</v>
+        <v>5.76867E-2</v>
       </c>
       <c r="K13" s="3">
-        <v>1.60905</v>
+        <v>1.6090500000000001</v>
       </c>
       <c r="L13" s="3">
-        <v>0.121121</v>
+        <v>0.12112100000000001</v>
       </c>
       <c r="M13" s="3">
-        <v>0.607002</v>
+        <v>0.60700200000000004</v>
       </c>
       <c r="N13" s="3">
-        <v>2.06015</v>
+        <v>2.0601500000000001</v>
       </c>
       <c r="O13" s="12">
-        <v>8.47846</v>
+        <v>8.4784600000000001</v>
       </c>
       <c r="P13" s="3">
-        <v>0.448093</v>
+        <v>0.44809300000000002</v>
       </c>
       <c r="Q13" s="26">
-        <v>44.8778</v>
+        <v>44.877800000000001</v>
       </c>
       <c r="R13" s="3">
-        <v>0.0175669</v>
+        <v>1.75669E-2</v>
       </c>
       <c r="S13" s="49">
-        <v>24.8271</v>
+        <v>24.827100000000002</v>
       </c>
       <c r="T13" s="3">
-        <v>29.3876</v>
+        <v>29.387599999999999</v>
       </c>
       <c r="U13" s="3">
-        <v>0.044533</v>
+        <v>4.4533000000000003E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>